<commit_message>
minor changes, and added a help file
</commit_message>
<xml_diff>
--- a/splitter/splitter.xlsx
+++ b/splitter/splitter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CTHOMBAR\Desktop\box\splitter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CTHOMBAR\Desktop\gt_rs\splitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8549C22F-4EC5-49C1-AEE6-0B81EE5D4A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC761508-AC77-45BE-BADC-6FBBB9082BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="0" windowWidth="17304" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,10 +118,10 @@
     <t>CHAKNA</t>
   </si>
   <si>
-    <t>A,C,D,H,J,P,R,S,V</t>
-  </si>
-  <si>
     <t>A, C, D, H, P, R, V</t>
+  </si>
+  <si>
+    <t>A,C,D,H,J,P, R,S,V</t>
   </si>
 </sst>
 </file>
@@ -603,7 +603,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,7 +623,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -693,7 +693,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>